<commit_message>
Updated field validation Test cases
Co-authored-by: Bhaveshgoldsmith <bhavesh.goldsmith@gmail.com>
Co-authored-by: mfaisalkhatri <mohammadfaisalkhatri@gmail.com>
</commit_message>
<xml_diff>
--- a/FieldValidation/TestCases_DropdownFieldValidation.xlsx
+++ b/FieldValidation/TestCases_DropdownFieldValidation.xlsx
@@ -258,11 +258,12 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B11"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="105.64"/>
   </cols>
   <sheetData>

</xml_diff>